<commit_message>
changed the display to dispaly the results
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLRandom.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLRandom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Random</t>
+  </si>
+  <si>
+    <t>buy</t>
   </si>
 </sst>
 </file>
@@ -113,9 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,7 +421,7 @@
     <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42627.87427083333</v>
       </c>
@@ -523,7 +527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42627.877280092594</v>
       </c>
@@ -574,6 +578,290 @@
       </c>
       <c r="Q3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42628.834120370368</v>
+      </c>
+      <c r="B4">
+        <v>-16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1.66</v>
+      </c>
+      <c r="S4" s="2">
+        <v>9.69E-2</v>
+      </c>
+      <c r="T4">
+        <v>4.57</v>
+      </c>
+      <c r="U4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V4">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42628.837546296294</v>
+      </c>
+      <c r="B5">
+        <v>-17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1.66</v>
+      </c>
+      <c r="S5" s="2">
+        <v>9.69E-2</v>
+      </c>
+      <c r="T5">
+        <v>4.57</v>
+      </c>
+      <c r="U5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V5">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42628.838750000003</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1.66</v>
+      </c>
+      <c r="S6" s="2">
+        <v>9.69E-2</v>
+      </c>
+      <c r="T6">
+        <v>4.57</v>
+      </c>
+      <c r="U6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V6">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42628.840949074074</v>
+      </c>
+      <c r="B7">
+        <v>-10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1.66</v>
+      </c>
+      <c r="S7" s="2">
+        <v>9.69E-2</v>
+      </c>
+      <c r="T7">
+        <v>4.57</v>
+      </c>
+      <c r="U7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V7">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>